<commit_message>
tutorial missions allmost there
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint 1/Burndown chart.xlsx
+++ b/Project_Management/Sprint 1/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GL704G\Desktop\freecol-SE-exercise\Project_Management\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13411498-9F55-4045-9030-4E676FD3BAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D5B4E7-033C-46AD-8C48-6DE379968212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -78,15 +78,6 @@
     <t>Ideal Burndown</t>
   </si>
   <si>
-    <t xml:space="preserve">Implement a round clock with 30s timer </t>
-  </si>
-  <si>
-    <t>Enlarge graphic zoom</t>
-  </si>
-  <si>
-    <t>Soldiers get a plus 1 movement unit when passing through sand</t>
-  </si>
-  <si>
     <t>Setup the FreeCol repository.</t>
   </si>
   <si>
@@ -94,18 +85,6 @@
   </si>
   <si>
     <t>Extract exhaustive information.</t>
-  </si>
-  <si>
-    <t>Identify metrics.</t>
-  </si>
-  <si>
-    <t>Design pattern identification.</t>
-  </si>
-  <si>
-    <t>Pinpoint code smells.</t>
-  </si>
-  <si>
-    <t>Compile reports (Metrics, GoF, Smells).</t>
   </si>
 </sst>
 </file>
@@ -2184,7 +2163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2305,7 +2284,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6" s="24">
         <v>1</v>
@@ -2325,7 +2304,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" s="25">
         <v>3</v>
@@ -2349,7 +2328,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="25">
         <v>4</v>
@@ -2371,15 +2350,9 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
-        <v>4</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="25">
-        <v>0</v>
-      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="11"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -2389,15 +2362,9 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="22">
-        <v>5</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="26">
-        <v>0</v>
-      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="12"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2407,15 +2374,9 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="22">
-        <v>6</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="26">
-        <v>0</v>
-      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="12"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -2425,15 +2386,9 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22">
-        <v>7</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="26">
-        <v>0</v>
-      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="12"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -2443,15 +2398,9 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
-        <v>8</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="26">
-        <v>0</v>
-      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="12"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -2461,15 +2410,9 @@
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="22">
-        <v>9</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="26">
-        <v>0</v>
-      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="12"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -2479,15 +2422,9 @@
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22">
-        <v>10</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="26">
-        <v>0</v>
-      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="26"/>
       <c r="E15" s="12"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>

</xml_diff>